<commit_message>
data files up to date:20 juin
</commit_message>
<xml_diff>
--- a/raw data/2021/Corona (76) copy 353.xlsx
+++ b/raw data/2021/Corona (76) copy 353.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhou/Desktop/CovidCasesQC/raw data/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DF4FEE-5025-A746-9A59-BEDB89A35EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32125F1F-B866-E84C-804F-8FBBA61D2EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="460" windowWidth="27320" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="1000" windowWidth="27320" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -480,7 +480,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>